<commit_message>
add send email system
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -21,7 +21,7 @@
     <author>Migiwa</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,30 +66,6 @@
           </rPr>
           <t xml:space="preserve">
 Pls show "MM/DD/YYYY"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-When user tick "Viet Nam", import "School Name" here.</t>
         </r>
       </text>
     </comment>
@@ -113,11 +89,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-When user tick "Nuoc ngoai", import "School Name" here.</t>
+When user tick "Viet Nam", import "School Name" here.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+When user tick "Nuoc ngoai", import "School Name" here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Gender</t>
   </si>
@@ -169,85 +169,73 @@
     <t>E-mail</t>
   </si>
   <si>
-    <t>Current Salary</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Expected Salary</t>
-  </si>
-  <si>
-    <t>Expected Industry</t>
-  </si>
-  <si>
-    <t>Expected Function</t>
-  </si>
-  <si>
-    <t>Expected Location</t>
-  </si>
-  <si>
-    <t>Expected job level</t>
-  </si>
-  <si>
-    <t>VN  School</t>
-  </si>
-  <si>
-    <t>Oversea School</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Graduation Year</t>
-  </si>
-  <si>
-    <t>Experienced Industry</t>
-  </si>
-  <si>
-    <t>Experienced Function</t>
-  </si>
-  <si>
-    <t>Experienced Job Level</t>
-  </si>
-  <si>
-    <t>Experience Year</t>
-  </si>
-  <si>
-    <t>Experience Details</t>
-  </si>
-  <si>
-    <t>Japanese level</t>
-  </si>
-  <si>
-    <t>English level</t>
-  </si>
-  <si>
-    <t>Vietnamese level</t>
-  </si>
-  <si>
-    <t>Other language proficiency</t>
-  </si>
-  <si>
-    <t>Skill</t>
-  </si>
-  <si>
-    <t>When change job?</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Birthday</t>
   </si>
   <si>
-    <t>Registration Date</t>
+    <t>Kana</t>
+  </si>
+  <si>
+    <t>Highest Degree</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Working Status</t>
+  </si>
+  <si>
+    <t>Number of companies</t>
+  </si>
+  <si>
+    <t>Function Category</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Annual Income</t>
+  </si>
+  <si>
+    <t>Industry Category</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Division Name</t>
+  </si>
+  <si>
+    <t>Job Contents</t>
+  </si>
+  <si>
+    <t>Job Descriptions</t>
+  </si>
+  <si>
+    <t>Other work history</t>
+  </si>
+  <si>
+    <t>Expected Industry Category</t>
+  </si>
+  <si>
+    <t>Expected Function Category</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>How can you know about company?</t>
+  </si>
+  <si>
+    <t>Number of employees</t>
+  </si>
+  <si>
+    <t>Worked Time</t>
   </si>
 </sst>
 </file>
@@ -290,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -313,14 +301,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,131 +627,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="27" max="27" width="17.85546875" customWidth="1"/>
-    <col min="29" max="29" width="24" customWidth="1"/>
-    <col min="36" max="36" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" customWidth="1"/>
+    <col min="21" max="22" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="21.28515625" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" customWidth="1"/>
+    <col min="28" max="28" width="26.28515625" customWidth="1"/>
+    <col min="29" max="29" width="19.42578125" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" customWidth="1"/>
+    <col min="31" max="31" width="38" customWidth="1"/>
+    <col min="32" max="32" width="24" customWidth="1"/>
+    <col min="39" max="39" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>19</v>
+      <c r="W1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AC1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AD1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AE1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -772,18 +789,21 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="AA2" s="3"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
     </row>
-    <row r="3" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix create-cv xcel file structure
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -27,18 +27,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t>Migiwa:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Pls show "Family Name + First Name"</t>
@@ -51,21 +49,41 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t>Migiwa:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Pls show "MM/DD/YYYY"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+When user tick "Viet Nam", import "School Name" here.</t>
         </r>
       </text>
     </comment>
@@ -75,69 +93,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t>Migiwa:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-When user tick "Viet Nam", import "School Name" here.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 When user tick "Nuoc ngoai", import "School Name" here.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-When user tick "I'm a fresh graduate", pls show the value of "Just Graduated/No work experience yet" in this field.</t>
         </r>
       </text>
     </comment>
@@ -146,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Gender</t>
   </si>
@@ -169,9 +137,6 @@
     <t>E-mail</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Birthday</t>
   </si>
   <si>
@@ -199,50 +164,50 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Annual Income</t>
-  </si>
-  <si>
     <t>Industry Category</t>
   </si>
   <si>
-    <t>Job Title</t>
-  </si>
-  <si>
-    <t>Division Name</t>
-  </si>
-  <si>
-    <t>Job Contents</t>
-  </si>
-  <si>
-    <t>Job Descriptions</t>
-  </si>
-  <si>
-    <t>Other work history</t>
-  </si>
-  <si>
-    <t>Expected Industry Category</t>
-  </si>
-  <si>
-    <t>Expected Function Category</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>How can you know about company?</t>
-  </si>
-  <si>
     <t>Number of employees</t>
   </si>
   <si>
     <t>Worked Time</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Annual Salary</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>Business Overview</t>
+  </si>
+  <si>
+    <t>Job Description</t>
+  </si>
+  <si>
+    <t>Other work experience</t>
+  </si>
+  <si>
+    <t>Expected Industry</t>
+  </si>
+  <si>
+    <t>Expected Function</t>
+  </si>
+  <si>
+    <t>Other Expectations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,17 +216,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -273,12 +236,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -301,31 +264,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +363,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -450,7 +397,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -626,144 +572,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" customWidth="1"/>
-    <col min="21" max="22" width="14.7109375" customWidth="1"/>
-    <col min="23" max="23" width="21.28515625" customWidth="1"/>
-    <col min="24" max="24" width="17.7109375" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17" customWidth="1"/>
-    <col min="27" max="27" width="17.7109375" customWidth="1"/>
-    <col min="28" max="28" width="26.28515625" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1"/>
-    <col min="31" max="31" width="38" customWidth="1"/>
-    <col min="32" max="32" width="24" customWidth="1"/>
-    <col min="39" max="39" width="17.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="2"/>
+    <col min="14" max="14" width="22.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="2" customWidth="1"/>
+    <col min="20" max="21" width="14.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="21.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="17" style="2" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="26.28515625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="19.42578125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="2" customWidth="1"/>
+    <col min="30" max="35" width="9.140625" style="2"/>
+    <col min="36" max="36" width="17.42578125" style="2" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:29">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
+      <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -789,21 +725,11 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="3"/>
+      <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
     </row>
-    <row r="3" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:29" ht="22.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -811,24 +737,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix create cv excel file
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -8,111 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Migiwa</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-Pls show "Family Name + First Name"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-Pls show "MM/DD/YYYY"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-When user tick "Viet Nam", import "School Name" here.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Migiwa:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-When user tick "Nuoc ngoai", import "School Name" here.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
@@ -176,9 +76,6 @@
     <t>Full Name</t>
   </si>
   <si>
-    <t>Annual Salary</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
@@ -201,30 +98,22 @@
   </si>
   <si>
     <t>Other Expectations</t>
+  </si>
+  <si>
+    <t>Monthly Salary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="3">
@@ -575,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,16 +548,16 @@
         <v>15</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>12</v>
@@ -680,22 +569,22 @@
         <v>18</v>
       </c>
       <c r="X1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -732,30 +621,5 @@
     <row r="3" spans="1:29" ht="22.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more fields on create-cv page
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Gender</t>
   </si>
@@ -101,6 +101,24 @@
   </si>
   <si>
     <t>Monthly Salary</t>
+  </si>
+  <si>
+    <t>English Level</t>
+  </si>
+  <si>
+    <t>Japanese Level</t>
+  </si>
+  <si>
+    <t>Other Language Proficiency</t>
+  </si>
+  <si>
+    <t>Expected Job Level</t>
+  </si>
+  <si>
+    <t>Expected Work Location</t>
+  </si>
+  <si>
+    <t>Expected Minimum Salary</t>
   </si>
 </sst>
 </file>
@@ -130,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -153,16 +171,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,16 +537,18 @@
     <col min="23" max="23" width="17.7109375" style="2" customWidth="1"/>
     <col min="24" max="24" width="14.28515625" style="2" customWidth="1"/>
     <col min="25" max="25" width="17" style="2" customWidth="1"/>
-    <col min="26" max="26" width="17.7109375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="26.28515625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="17.85546875" style="2" customWidth="1"/>
-    <col min="30" max="35" width="9.140625" style="2"/>
-    <col min="36" max="36" width="17.42578125" style="2" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="2"/>
+    <col min="26" max="26" width="21.85546875" style="2" customWidth="1"/>
+    <col min="27" max="28" width="17.7109375" style="2" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="26.28515625" style="2" customWidth="1"/>
+    <col min="31" max="34" width="19.42578125" style="2" customWidth="1"/>
+    <col min="35" max="35" width="17.85546875" style="2" customWidth="1"/>
+    <col min="36" max="41" width="9.140625" style="2"/>
+    <col min="42" max="42" width="17.42578125" style="2" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:35">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -577,17 +627,35 @@
       <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AF1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -617,8 +685,14 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:29" ht="22.5" customHeight="1"/>
+    <row r="3" spans="1:35" ht="22.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix create CV page
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -100,9 +100,6 @@
     <t>Other Expectations</t>
   </si>
   <si>
-    <t>Monthly Salary</t>
-  </si>
-  <si>
     <t>English Level</t>
   </si>
   <si>
@@ -118,7 +115,10 @@
     <t>Expected Work Location</t>
   </si>
   <si>
-    <t>Expected Minimum Salary</t>
+    <t>Expected Minimum Salary (万円)</t>
+  </si>
+  <si>
+    <t>Monthly Salary (万円)</t>
   </si>
 </sst>
 </file>
@@ -134,18 +134,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -203,12 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -512,36 +505,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="15.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="14.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
     <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="18.140625" style="2" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="2"/>
     <col min="14" max="14" width="22.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="18.7109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="15" style="2" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
     <col min="19" max="19" width="8.85546875" style="2" customWidth="1"/>
     <col min="20" max="21" width="14.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="21.28515625" style="2" customWidth="1"/>
     <col min="23" max="23" width="17.7109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="19.140625" style="2" customWidth="1"/>
     <col min="25" max="25" width="17" style="2" customWidth="1"/>
     <col min="26" max="26" width="21.85546875" style="2" customWidth="1"/>
     <col min="27" max="28" width="17.7109375" style="2" customWidth="1"/>
     <col min="29" max="29" width="25.28515625" style="2" customWidth="1"/>
     <col min="30" max="30" width="26.28515625" style="2" customWidth="1"/>
-    <col min="31" max="34" width="19.42578125" style="2" customWidth="1"/>
+    <col min="31" max="32" width="19.42578125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="22.28515625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="31.7109375" style="2" customWidth="1"/>
     <col min="35" max="35" width="17.85546875" style="2" customWidth="1"/>
     <col min="36" max="41" width="9.140625" style="2"/>
     <col min="42" max="42" width="17.42578125" style="2" customWidth="1"/>
@@ -597,8 +595,8 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>28</v>
+      <c r="Q1" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>16</v>
@@ -627,14 +625,14 @@
       <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>25</v>
@@ -642,14 +640,14 @@
       <c r="AE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="AI1" s="3" t="s">
         <v>27</v>

</xml_diff>